<commit_message>
Small fix for 10 and 11 tasks
</commit_message>
<xml_diff>
--- a/Task_11_language_models/ndgc_calc.xlsx
+++ b/Task_11_language_models/ndgc_calc.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mvideo\Dropbox\Edu\Semestr_M3\Information Retrieval\Task_11_language_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dropbox\Edu\Semestr_M3\Information Retrieval\Task_11_language_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="4800" windowWidth="21600" windowHeight="11400"/>
+    <workbookView xWindow="3108" yWindow="4800" windowWidth="21600" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>i</t>
   </si>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,13 +388,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,20 +428,20 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <f>B3/(LOG(A3+1,2))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <f>SUM(C$3:C3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -456,29 +456,29 @@
       </c>
       <c r="H3">
         <f>D3/G3</f>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C8" si="0">B4/(LOG(A4+1,2))</f>
-        <v>1.2618595071429148</v>
+        <f t="shared" ref="C4:C5" si="0">B4/(LOG(A4+1,2))</f>
+        <v>2.5237190142858297</v>
       </c>
       <c r="D4">
         <f>SUM(C$3:C4)</f>
-        <v>4.2618595071429146</v>
+        <v>3.5237190142858297</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F7" si="1">E4/(LOG(A4+1,2))</f>
+        <f t="shared" ref="F4:F5" si="1">E4/(LOG(A4+1,2))</f>
         <v>2.5237190142858297</v>
       </c>
       <c r="G4">
@@ -486,11 +486,11 @@
         <v>7.5237190142858292</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H8" si="2">D4/G4</f>
-        <v>0.56645649565734901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H4:H5" si="2">D4/G4</f>
+        <v>0.4683480347412084</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -503,7 +503,7 @@
       </c>
       <c r="D5">
         <f>SUM(C$3:C5)</f>
-        <v>5.2618595071429146</v>
+        <v>4.5237190142858292</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -517,364 +517,50 @@
         <v>9.0237190142858292</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
-        <v>0.58311429010728766</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <f>B8/(LOG(A8+1,2))</f>
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <f>SUM(C$3:C8)</f>
-        <v>6.2618595071429146</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <f>E8/(LOG(A8+1,2))</f>
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <f>SUM(F$3:F8)</f>
-        <v>14.023719014285829</v>
-      </c>
-      <c r="H8">
-        <f>D8/G8</f>
-        <v>0.44651917945332603</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <f>K8/(LOG(J8+1,2))</f>
-        <v>1</v>
-      </c>
-      <c r="M8">
-        <f>SUM(L$3:L8)</f>
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>5</v>
-      </c>
-      <c r="O8">
-        <f>N8/(LOG(J8+1,2))</f>
-        <v>5</v>
-      </c>
-      <c r="P8">
-        <f>SUM(O$3:O8)</f>
-        <v>5</v>
-      </c>
-      <c r="Q8">
-        <f>M8/P8</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:C10" si="3">B9/(LOG(A9+1,2))</f>
-        <v>1.2618595071429148</v>
-      </c>
-      <c r="D9">
-        <f>SUM(C$3:C9)</f>
-        <v>7.5237190142858292</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F10" si="4">E9/(LOG(A9+1,2))</f>
-        <v>2.5237190142858297</v>
-      </c>
-      <c r="G9">
-        <f>SUM(F$3:F9)</f>
-        <v>16.547438028571658</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ref="H9:H10" si="5">D9/G9</f>
-        <v>0.45467576317826291</v>
-      </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>4</v>
-      </c>
-      <c r="L9">
-        <f t="shared" ref="L9:L10" si="6">K9/(LOG(J9+1,2))</f>
-        <v>2.5237190142858297</v>
-      </c>
-      <c r="M9">
-        <f>SUM(L$3:L9)</f>
-        <v>3.5237190142858297</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <f t="shared" ref="O9:O10" si="7">N9/(LOG(J9+1,2))</f>
-        <v>2.5237190142858297</v>
-      </c>
-      <c r="P9">
-        <f>SUM(O$3:O9)</f>
-        <v>7.5237190142858292</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" ref="Q9:Q10" si="8">M9/P9</f>
-        <v>0.4683480347412084</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <f>SUM(C$3:C10)</f>
-        <v>8.5237190142858292</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="4"/>
-        <v>1.5</v>
-      </c>
-      <c r="G10">
-        <f>SUM(F$3:F10)</f>
-        <v>18.047438028571658</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="5"/>
-        <v>0.47229523663090411</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <f>SUM(L$3:L10)</f>
-        <v>4.5237190142858292</v>
-      </c>
-      <c r="N10">
-        <v>3</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="7"/>
-        <v>1.5</v>
-      </c>
-      <c r="P10">
-        <f>SUM(O$3:O10)</f>
-        <v>9.0237190142858292</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="8"/>
+        <f>D5/G5</f>
         <v>0.50131425935627416</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <f>B13/(LOG(A13+1,2))</f>
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <f>SUM(C$3:C13)</f>
-        <v>10.523719014285829</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <f>E13/(LOG(A13+1,2))</f>
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <f>SUM(F$3:F13)</f>
-        <v>23.047438028571658</v>
-      </c>
-      <c r="H13">
-        <f>D13/G13</f>
-        <v>0.45661122946679317</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:C15" si="9">B14/(LOG(A14+1,2))</f>
-        <v>0.63092975357145742</v>
-      </c>
-      <c r="D14">
-        <f>SUM(C$3:C14)</f>
-        <v>11.154648767857287</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="F14:F15" si="10">E14/(LOG(A14+1,2))</f>
-        <v>2.5237190142858297</v>
-      </c>
-      <c r="G14">
-        <f>SUM(F$3:F14)</f>
-        <v>25.571157042857489</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ref="H14:H15" si="11">D14/G14</f>
-        <v>0.43621994691761484</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <f>SUM(C$3:C15)</f>
-        <v>11.154648767857287</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="G15">
-        <f>SUM(F$3:F15)</f>
-        <v>27.071157042857489</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="11"/>
-        <v>0.41204920610515067</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H18" s="2"/>
     </row>
   </sheetData>

</xml_diff>